<commit_message>
fix excel export and tests
</commit_message>
<xml_diff>
--- a/cases/0-hello-world/master/table.xlsx
+++ b/cases/0-hello-world/master/table.xlsx
@@ -7,8 +7,7 @@
     <sheet name="Species" sheetId="2" r:id="rId2"/>
     <sheet name="Reaction" sheetId="3" r:id="rId3"/>
     <sheet name="Const" sheetId="4" r:id="rId4"/>
-    <sheet name="UnitDef" sheetId="5" r:id="rId5"/>
-    <sheet name="undefined" sheetId="6" r:id="rId6"/>
+    <sheet name="undefined" sheetId="5" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
@@ -601,7 +600,7 @@
         <v>Vmax * S / (Km + S) * default_comp</v>
       </c>
       <c r="F2" t="str">
-        <v>umole/min</v>
+        <v>umole/minute</v>
       </c>
       <c r="G2" t="str">
         <v>S = P</v>
@@ -696,7 +695,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -706,7 +705,7 @@
         <v>on</v>
       </c>
       <c r="B1" t="str">
-        <v>class</v>
+        <v>action</v>
       </c>
       <c r="C1" t="str">
         <v>space</v>
@@ -717,22 +716,22 @@
       <c r="E1" t="str">
         <v>units</v>
       </c>
+      <c r="F1" t="str">
+        <v>type</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>UnitDef</v>
+        <v>setNS</v>
       </c>
       <c r="C2" t="str">
         <v>mm</v>
       </c>
-      <c r="D2" t="str">
-        <v>fmole</v>
-      </c>
-      <c r="E2" t="str">
-        <v>(1e-15 mole)</v>
+      <c r="F2" t="str">
+        <v>concrete</v>
       </c>
     </row>
     <row r="3">
@@ -740,16 +739,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C3" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D3" t="str">
-        <v>pmole</v>
+        <v>fmole</v>
       </c>
       <c r="E3" t="str">
-        <v>(1e-12 mole)</v>
+        <v>(1e-15 mole)</v>
       </c>
     </row>
     <row r="4">
@@ -757,16 +753,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C4" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D4" t="str">
-        <v>nmole</v>
+        <v>pmole</v>
       </c>
       <c r="E4" t="str">
-        <v>(1e-9 mole)</v>
+        <v>(1e-12 mole)</v>
       </c>
     </row>
     <row r="5">
@@ -774,16 +767,13 @@
         <v>1</v>
       </c>
       <c r="B5" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C5" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D5" t="str">
-        <v>umole</v>
+        <v>nmole</v>
       </c>
       <c r="E5" t="str">
-        <v>(1e-6 mole)</v>
+        <v>(1e-9 mole)</v>
       </c>
     </row>
     <row r="6">
@@ -791,16 +781,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C6" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D6" t="str">
-        <v>mmole</v>
+        <v>umole</v>
       </c>
       <c r="E6" t="str">
-        <v>(1e-3 mole)</v>
+        <v>(1e-6 mole)</v>
       </c>
     </row>
     <row r="7">
@@ -808,16 +795,13 @@
         <v>1</v>
       </c>
       <c r="B7" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C7" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D7" t="str">
-        <v>fM</v>
+        <v>mmole</v>
       </c>
       <c r="E7" t="str">
-        <v>(1e-15 mole)/litre</v>
+        <v>(1e-3 mole)</v>
       </c>
     </row>
     <row r="8">
@@ -825,16 +809,13 @@
         <v>1</v>
       </c>
       <c r="B8" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C8" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D8" t="str">
-        <v>pM</v>
+        <v>fM</v>
       </c>
       <c r="E8" t="str">
-        <v>(1e-12 mole)/litre</v>
+        <v>(1e-15 mole)/litre</v>
       </c>
     </row>
     <row r="9">
@@ -842,16 +823,13 @@
         <v>1</v>
       </c>
       <c r="B9" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C9" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D9" t="str">
-        <v>nM</v>
+        <v>pM</v>
       </c>
       <c r="E9" t="str">
-        <v>(1e-9 mole)/litre</v>
+        <v>(1e-12 mole)/litre</v>
       </c>
     </row>
     <row r="10">
@@ -859,16 +837,13 @@
         <v>1</v>
       </c>
       <c r="B10" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C10" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D10" t="str">
-        <v>uM</v>
+        <v>nM</v>
       </c>
       <c r="E10" t="str">
-        <v>(1e-6 mole)/litre</v>
+        <v>(1e-9 mole)/litre</v>
       </c>
     </row>
     <row r="11">
@@ -876,16 +851,13 @@
         <v>1</v>
       </c>
       <c r="B11" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C11" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D11" t="str">
-        <v>mM</v>
+        <v>uM</v>
       </c>
       <c r="E11" t="str">
-        <v>(1e-3 mole)/litre</v>
+        <v>(1e-6 mole)/litre</v>
       </c>
     </row>
     <row r="12">
@@ -893,16 +865,13 @@
         <v>1</v>
       </c>
       <c r="B12" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C12" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D12" t="str">
-        <v>M</v>
+        <v>mM</v>
       </c>
       <c r="E12" t="str">
-        <v>mole/litre</v>
+        <v>(1e-3 mole)/litre</v>
       </c>
     </row>
     <row r="13">
@@ -910,16 +879,13 @@
         <v>1</v>
       </c>
       <c r="B13" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C13" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D13" t="str">
-        <v>kM</v>
+        <v>M</v>
       </c>
       <c r="E13" t="str">
-        <v>(1e+3 mole)/litre</v>
+        <v>mole/litre</v>
       </c>
     </row>
     <row r="14">
@@ -927,16 +893,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C14" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D14" t="str">
-        <v>fL</v>
+        <v>kM</v>
       </c>
       <c r="E14" t="str">
-        <v>(1e-15 litre)</v>
+        <v>(1e+3 mole)/litre</v>
       </c>
     </row>
     <row r="15">
@@ -944,16 +907,13 @@
         <v>1</v>
       </c>
       <c r="B15" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C15" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D15" t="str">
-        <v>pL</v>
+        <v>fL</v>
       </c>
       <c r="E15" t="str">
-        <v>(1e-12 litre)</v>
+        <v>(1e-15 litre)</v>
       </c>
     </row>
     <row r="16">
@@ -961,16 +921,13 @@
         <v>1</v>
       </c>
       <c r="B16" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C16" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D16" t="str">
-        <v>nL</v>
+        <v>pL</v>
       </c>
       <c r="E16" t="str">
-        <v>(1e-9 litre)</v>
+        <v>(1e-12 litre)</v>
       </c>
     </row>
     <row r="17">
@@ -978,16 +935,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C17" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D17" t="str">
-        <v>uL</v>
+        <v>nL</v>
       </c>
       <c r="E17" t="str">
-        <v>(1e-6 litre)</v>
+        <v>(1e-9 litre)</v>
       </c>
     </row>
     <row r="18">
@@ -995,16 +949,13 @@
         <v>1</v>
       </c>
       <c r="B18" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C18" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D18" t="str">
-        <v>mL</v>
+        <v>uL</v>
       </c>
       <c r="E18" t="str">
-        <v>(1e-3 litre)</v>
+        <v>(1e-6 litre)</v>
       </c>
     </row>
     <row r="19">
@@ -1012,16 +963,13 @@
         <v>1</v>
       </c>
       <c r="B19" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C19" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D19" t="str">
-        <v>dL</v>
+        <v>mL</v>
       </c>
       <c r="E19" t="str">
-        <v>(1e-1 litre)</v>
+        <v>(1e-3 litre)</v>
       </c>
     </row>
     <row r="20">
@@ -1029,16 +977,13 @@
         <v>1</v>
       </c>
       <c r="B20" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C20" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D20" t="str">
-        <v>L</v>
+        <v>dL</v>
       </c>
       <c r="E20" t="str">
-        <v>litre</v>
+        <v>(1e-1 litre)</v>
       </c>
     </row>
     <row r="21">
@@ -1046,16 +991,13 @@
         <v>1</v>
       </c>
       <c r="B21" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C21" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D21" t="str">
-        <v>fs</v>
+        <v>L</v>
       </c>
       <c r="E21" t="str">
-        <v>(1e-15 second)</v>
+        <v>litre</v>
       </c>
     </row>
     <row r="22">
@@ -1063,16 +1005,13 @@
         <v>1</v>
       </c>
       <c r="B22" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C22" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D22" t="str">
-        <v>ps</v>
+        <v>fs</v>
       </c>
       <c r="E22" t="str">
-        <v>(1e-12 second)</v>
+        <v>(1e-15 second)</v>
       </c>
     </row>
     <row r="23">
@@ -1080,16 +1019,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C23" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D23" t="str">
-        <v>ns</v>
+        <v>ps</v>
       </c>
       <c r="E23" t="str">
-        <v>(1e-9 second)</v>
+        <v>(1e-12 second)</v>
       </c>
     </row>
     <row r="24">
@@ -1097,16 +1033,13 @@
         <v>1</v>
       </c>
       <c r="B24" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C24" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D24" t="str">
-        <v>us</v>
+        <v>ns</v>
       </c>
       <c r="E24" t="str">
-        <v>(1e-6 second)</v>
+        <v>(1e-9 second)</v>
       </c>
     </row>
     <row r="25">
@@ -1114,16 +1047,13 @@
         <v>1</v>
       </c>
       <c r="B25" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C25" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D25" t="str">
-        <v>ms</v>
+        <v>us</v>
       </c>
       <c r="E25" t="str">
-        <v>(1e-3 second)</v>
+        <v>(1e-6 second)</v>
       </c>
     </row>
     <row r="26">
@@ -1131,16 +1061,13 @@
         <v>1</v>
       </c>
       <c r="B26" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C26" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D26" t="str">
-        <v>s</v>
+        <v>ms</v>
       </c>
       <c r="E26" t="str">
-        <v>second</v>
+        <v>(1e-3 second)</v>
       </c>
     </row>
     <row r="27">
@@ -1148,16 +1075,13 @@
         <v>1</v>
       </c>
       <c r="B27" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C27" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D27" t="str">
-        <v>min</v>
+        <v>s</v>
       </c>
       <c r="E27" t="str">
-        <v>(6e+1 second)</v>
+        <v>second</v>
       </c>
     </row>
     <row r="28">
@@ -1165,16 +1089,13 @@
         <v>1</v>
       </c>
       <c r="B28" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C28" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D28" t="str">
         <v>h</v>
       </c>
       <c r="E28" t="str">
-        <v>(3.6e+3 second)</v>
+        <v>hour</v>
       </c>
     </row>
     <row r="29">
@@ -1182,16 +1103,13 @@
         <v>1</v>
       </c>
       <c r="B29" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C29" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D29" t="str">
         <v>week</v>
       </c>
       <c r="E29" t="str">
-        <v>(6.048e+5 second)</v>
+        <v>(7e+0 day)</v>
       </c>
     </row>
     <row r="30">
@@ -1199,10 +1117,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C30" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D30" t="str">
         <v>fg</v>
@@ -1216,10 +1131,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C31" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D31" t="str">
         <v>pg</v>
@@ -1233,10 +1145,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C32" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D32" t="str">
         <v>ng</v>
@@ -1250,10 +1159,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C33" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D33" t="str">
         <v>ug</v>
@@ -1267,10 +1173,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C34" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D34" t="str">
         <v>mg</v>
@@ -1284,10 +1187,7 @@
         <v>1</v>
       </c>
       <c r="B35" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C35" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D35" t="str">
         <v>g</v>
@@ -1301,10 +1201,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C36" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D36" t="str">
         <v>kg</v>
@@ -1318,10 +1215,7 @@
         <v>1</v>
       </c>
       <c r="B37" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C37" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D37" t="str">
         <v>kat</v>
@@ -1335,10 +1229,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C38" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D38" t="str">
         <v>cell</v>
@@ -1352,10 +1243,7 @@
         <v>1</v>
       </c>
       <c r="B39" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C39" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D39" t="str">
         <v>kcell</v>
@@ -1369,10 +1257,7 @@
         <v>1</v>
       </c>
       <c r="B40" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C40" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D40" t="str">
         <v>cal</v>
@@ -1386,10 +1271,7 @@
         <v>1</v>
       </c>
       <c r="B41" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C41" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D41" t="str">
         <v>kcal</v>
@@ -1403,10 +1285,7 @@
         <v>1</v>
       </c>
       <c r="B42" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C42" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D42" t="str">
         <v>fm</v>
@@ -1420,10 +1299,7 @@
         <v>1</v>
       </c>
       <c r="B43" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C43" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D43" t="str">
         <v>pm</v>
@@ -1437,10 +1313,7 @@
         <v>1</v>
       </c>
       <c r="B44" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C44" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D44" t="str">
         <v>nm</v>
@@ -1454,10 +1327,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C45" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D45" t="str">
         <v>um</v>
@@ -1471,10 +1341,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C46" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D46" t="str">
         <v>mm</v>
@@ -1488,10 +1355,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C47" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D47" t="str">
         <v>cm</v>
@@ -1505,10 +1369,7 @@
         <v>1</v>
       </c>
       <c r="B48" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C48" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D48" t="str">
         <v>m</v>
@@ -1522,10 +1383,7 @@
         <v>1</v>
       </c>
       <c r="B49" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C49" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D49" t="str">
         <v>UL</v>
@@ -1539,10 +1397,7 @@
         <v>1</v>
       </c>
       <c r="B50" t="str">
-        <v>UnitDef</v>
-      </c>
-      <c r="C50" t="str">
-        <v>mm</v>
+        <v>defineUnit</v>
       </c>
       <c r="D50" t="str">
         <v>percent</v>
@@ -1553,49 +1408,7 @@
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E50"/>
-  </ignoredErrors>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>on</v>
-      </c>
-      <c r="B1" t="str">
-        <v>action</v>
-      </c>
-      <c r="C1" t="str">
-        <v>space</v>
-      </c>
-      <c r="D1" t="str">
-        <v>type</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>setNS</v>
-      </c>
-      <c r="C2" t="str">
-        <v>mm</v>
-      </c>
-      <c r="D2" t="str">
-        <v>concrete</v>
-      </c>
-    </row>
-  </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>